<commit_message>
Source and id parsing update
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E86"/>
+  <dimension ref="A1:H86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +438,9 @@
     <col width="16" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
     <col width="13" customWidth="1" min="5" max="5"/>
+    <col width="9" customWidth="1" min="6" max="6"/>
+    <col width="8" customWidth="1" min="7" max="7"/>
+    <col width="6" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -466,6 +469,21 @@
           <t>Type</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>ECO</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Source</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -489,6 +507,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2MIO</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -512,6 +545,21 @@
           <t>Beta strand</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2MIO</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -535,6 +583,21 @@
           <t>Beta strand</t>
         </is>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2MIO</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -558,6 +621,21 @@
           <t>Beta strand</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2MIO</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -581,6 +659,21 @@
           <t>Beta strand</t>
         </is>
       </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2MIO</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -604,6 +697,21 @@
           <t>Beta strand</t>
         </is>
       </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2MIO</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -627,6 +735,21 @@
           <t>Beta strand</t>
         </is>
       </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2MIO</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -650,6 +773,21 @@
           <t>Beta strand</t>
         </is>
       </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2MIO</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -673,6 +811,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>6Y7F</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -696,6 +849,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>6Y7F</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -719,6 +887,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>6Y7F</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -742,6 +925,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>6Y7F</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -765,6 +963,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>6Y7F</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -788,6 +1001,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>6Y7F</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -811,6 +1039,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>6Y7F</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -834,6 +1077,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>6Y7F</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -857,6 +1115,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>6Y7F</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -880,6 +1153,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>6Y7F</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -903,6 +1191,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>6Y7F</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -926,6 +1229,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>6Y7F</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -949,6 +1267,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>6Y7F</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -972,6 +1305,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>6Y7F</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -995,6 +1343,21 @@
           <t>Turn</t>
         </is>
       </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>6Y7F</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1018,6 +1381,21 @@
           <t>Beta strand</t>
         </is>
       </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>6Y7F</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1041,6 +1419,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>3AL5</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1064,6 +1457,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>3AL5</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1087,6 +1495,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>3AL5</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1110,6 +1533,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>3AL5</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1133,6 +1571,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>3AL5</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1156,6 +1609,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>3AL5</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1179,6 +1647,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>3AL5</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1202,6 +1685,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>3AL5</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1225,6 +1723,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>3AL5</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1248,6 +1761,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>3AL5</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1271,6 +1799,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>3AL5</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1294,6 +1837,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>3AL5</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1317,6 +1875,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>3AL5</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1340,6 +1913,21 @@
           <t>Turn</t>
         </is>
       </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>3AL6</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1363,6 +1951,21 @@
           <t>Turn</t>
         </is>
       </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>3AL5</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1386,6 +1989,21 @@
           <t>Turn</t>
         </is>
       </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>3AL5</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1409,6 +2027,21 @@
           <t>Beta strand</t>
         </is>
       </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>3AL5</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1432,6 +2065,21 @@
           <t>Beta strand</t>
         </is>
       </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>3AL5</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1455,6 +2103,21 @@
           <t>Beta strand</t>
         </is>
       </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>3AL5</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1478,6 +2141,21 @@
           <t>Beta strand</t>
         </is>
       </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>3AL5</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1501,6 +2179,21 @@
           <t>Beta strand</t>
         </is>
       </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>3AL5</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1524,6 +2217,21 @@
           <t>Beta strand</t>
         </is>
       </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>3AL5</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1547,6 +2255,21 @@
           <t>Beta strand</t>
         </is>
       </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>3AL5</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1570,6 +2293,21 @@
           <t>Beta strand</t>
         </is>
       </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>3AL5</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1593,6 +2331,21 @@
           <t>Beta strand</t>
         </is>
       </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>3AL5</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1616,6 +2369,21 @@
           <t>Beta strand</t>
         </is>
       </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>3AL5</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1639,6 +2407,21 @@
           <t>Beta strand</t>
         </is>
       </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>3AL5</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1662,6 +2445,21 @@
           <t>Beta strand</t>
         </is>
       </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>3AL5</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1685,6 +2483,21 @@
           <t>Beta strand</t>
         </is>
       </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>3AL5</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1708,6 +2521,21 @@
           <t>Beta strand</t>
         </is>
       </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>3AL5</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1731,6 +2559,21 @@
           <t>Beta strand</t>
         </is>
       </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>3AL5</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1754,6 +2597,21 @@
           <t>Beta strand</t>
         </is>
       </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>3AL5</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1777,6 +2635,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>7F6L</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1800,6 +2673,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>7F6L</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1823,6 +2711,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>7F6L</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1846,6 +2749,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>7F6L</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1869,6 +2787,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>7F6L</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1892,6 +2825,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>7F6L</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1915,6 +2863,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>7F6L</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1938,6 +2901,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>7F6L</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1961,6 +2939,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>7F6L</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1984,6 +2977,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>7F6L</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2007,6 +3015,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>7F6L</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2030,6 +3053,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>7F6L</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2053,6 +3091,21 @@
           <t>Turn</t>
         </is>
       </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>7F6L</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2076,6 +3129,21 @@
           <t>Turn</t>
         </is>
       </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>7F6L</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2099,6 +3167,21 @@
           <t>Beta strand</t>
         </is>
       </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>7F6L</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2122,6 +3205,21 @@
           <t>Beta strand</t>
         </is>
       </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>7F6L</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2145,6 +3243,21 @@
           <t>Beta strand</t>
         </is>
       </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>7F6L</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2168,6 +3281,21 @@
           <t>Beta strand</t>
         </is>
       </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>7F6L</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2191,6 +3319,21 @@
           <t>Beta strand</t>
         </is>
       </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>7F6L</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -2214,6 +3357,21 @@
           <t>Beta strand</t>
         </is>
       </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>7F6L</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2237,6 +3395,21 @@
           <t>Beta strand</t>
         </is>
       </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>7F6L</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2260,6 +3433,21 @@
           <t>Beta strand</t>
         </is>
       </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>7F6L</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -2283,6 +3471,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>5N9G</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -2306,6 +3509,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>5N9G</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -2329,6 +3547,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>5N9G</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -2352,6 +3585,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>5N9G</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -2375,6 +3623,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>5N9G</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -2398,6 +3661,21 @@
           <t>Helix</t>
         </is>
       </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>7LXF</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -2419,6 +3697,21 @@
       <c r="E86" t="inlineStr">
         <is>
           <t>Helix</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>0007829</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>PDB</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>7LXF</t>
         </is>
       </c>
     </row>

</xml_diff>